<commit_message>
Changed name to part1cb3
</commit_message>
<xml_diff>
--- a/20200929_Assesment1a_Analytical_DesignOp_EA.xlsx
+++ b/20200929_Assesment1a_Analytical_DesignOp_EA.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/2326f21fcfb2723d/Projects/UoB 4th Year/Design Optimisation Project/Design Optimisation Skills/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ege\Documents\GitHub\Design-Optimisation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="686" documentId="11_F25DC773A252ABDACC1048B7615F43B25BDE58E0" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{221C0706-8A03-4F76-9635-F654534B9F63}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{E2B198A6-243E-48D7-8BE9-D4CE86A8B335}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -200,7 +200,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="167" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -339,12 +339,8 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="2"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="1" applyFont="1" applyAlignment="1">
@@ -353,43 +349,43 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -404,38 +400,7 @@
     <cellStyle name="Input" xfId="1" builtinId="20"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -540,16 +505,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>517871</xdr:colOff>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>47224</xdr:colOff>
       <xdr:row>30</xdr:row>
-      <xdr:rowOff>21612</xdr:rowOff>
+      <xdr:rowOff>55230</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>276864</xdr:colOff>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>411335</xdr:colOff>
       <xdr:row>33</xdr:row>
-      <xdr:rowOff>31137</xdr:rowOff>
+      <xdr:rowOff>64755</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -579,8 +544,8 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="6913228" y="5736612"/>
-          <a:ext cx="4045242" cy="581025"/>
+          <a:off x="16878459" y="5770230"/>
+          <a:ext cx="3994817" cy="581025"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -603,16 +568,16 @@
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
-          <xdr:col>4</xdr:col>
-          <xdr:colOff>0</xdr:colOff>
-          <xdr:row>1</xdr:row>
-          <xdr:rowOff>0</xdr:rowOff>
+          <xdr:col>23</xdr:col>
+          <xdr:colOff>224117</xdr:colOff>
+          <xdr:row>11</xdr:row>
+          <xdr:rowOff>67236</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>10</xdr:col>
-          <xdr:colOff>561975</xdr:colOff>
-          <xdr:row>19</xdr:row>
-          <xdr:rowOff>9525</xdr:rowOff>
+          <xdr:col>30</xdr:col>
+          <xdr:colOff>201705</xdr:colOff>
+          <xdr:row>29</xdr:row>
+          <xdr:rowOff>67236</xdr:rowOff>
         </xdr:to>
         <xdr:pic>
           <xdr:nvPicPr>
@@ -627,7 +592,7 @@
               <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
               <a:extLst>
                 <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
-                  <a14:cameraTool cellRange="$B$1:$C$18" spid="_x0000_s1029"/>
+                  <a14:cameraTool cellRange="$B$1:$C$18" spid="_x0000_s1032"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPicPr>
@@ -641,8 +606,8 @@
           </xdr:blipFill>
           <xdr:spPr bwMode="auto">
             <a:xfrm>
-              <a:off x="5334000" y="190500"/>
-              <a:ext cx="4219575" cy="3438525"/>
+              <a:off x="17055352" y="2162736"/>
+              <a:ext cx="4213412" cy="3429000"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -664,6 +629,67 @@
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>33618</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>134470</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>595593</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>143995</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A581C2E0-EE80-474F-ADAF-1B1F28021599}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="13839265" y="6420970"/>
+          <a:ext cx="4192681" cy="4200525"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -930,10 +956,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:E32"/>
+  <dimension ref="B1:E22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -944,188 +970,184 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="7">
+      <c r="C1" s="5">
         <f>C2*C3*C4</f>
         <v>384555119.38424003</v>
       </c>
-      <c r="E1" s="3"/>
+      <c r="E1" s="1"/>
     </row>
     <row r="2" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="9">
+      <c r="C2" s="7">
         <v>828.67700000000002</v>
       </c>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="9">
+      <c r="C3" s="7">
         <v>828.67700000000002</v>
       </c>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="9">
+      <c r="C4" s="7">
         <v>560</v>
       </c>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B5" s="10" t="s">
+      <c r="B5" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="11">
+      <c r="C5" s="9">
         <f>PI()*((C6)^2)*C7</f>
         <v>500000</v>
       </c>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B6" s="12" t="s">
+      <c r="B6" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="13">
+      <c r="C6" s="11">
         <v>33.1</v>
       </c>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B7" s="12" t="s">
+      <c r="B7" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="13">
+      <c r="C7" s="11">
         <f>(500000)/(PI()*(C6)^2)</f>
         <v>145.26605552331151</v>
       </c>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B8" s="12" t="s">
+      <c r="B8" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="13">
+      <c r="C8" s="11">
         <v>11</v>
       </c>
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B9" s="12" t="s">
+      <c r="B9" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="13">
+      <c r="C9" s="11">
         <f>(2*C8+1+SQRT(3))/SQRT(3)</f>
         <v>14.279056191361395</v>
       </c>
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B10" s="14" t="s">
+      <c r="B10" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="15">
+      <c r="C10" s="13">
         <f>(2*C8+1)*C6</f>
         <v>761.30000000000007</v>
       </c>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B11" s="14" t="s">
+      <c r="B11" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="C11" s="15">
+      <c r="C11" s="13">
         <f>(2+(C9-1)*SQRT(3))*C6</f>
         <v>827.50000000000011</v>
       </c>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B12" s="14" t="s">
+      <c r="B12" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="C12" s="15">
+      <c r="C12" s="13">
         <f>C13*C7</f>
         <v>560</v>
       </c>
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B13" s="10" t="s">
+      <c r="B13" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="C13" s="11">
+      <c r="C13" s="9">
         <f>C4/C7</f>
         <v>3.8549955664634554</v>
       </c>
     </row>
     <row r="14" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B14" s="10" t="s">
+      <c r="B14" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="C14" s="11">
+      <c r="C14" s="9">
         <f>C8*C9*C13</f>
         <v>605.50268142078801</v>
       </c>
     </row>
     <row r="15" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B15" s="10" t="s">
+      <c r="B15" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="C15" s="11">
+      <c r="C15" s="9">
         <f>C14*C5</f>
         <v>302751340.71039402</v>
       </c>
     </row>
     <row r="16" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B16" s="16" t="s">
+      <c r="B16" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="C16" s="17">
+      <c r="C16" s="15">
         <f>C15/C1</f>
         <v>0.78727684394155928</v>
       </c>
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B17" s="18" t="s">
+      <c r="B17" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="C17" s="19">
+      <c r="C17" s="17">
         <f>PI()/(2*SQRT(3))</f>
         <v>0.90689968211710892</v>
       </c>
     </row>
     <row r="18" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B18" s="20" t="s">
+      <c r="B18" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="C18" s="21">
+      <c r="C18" s="19">
         <f>C1*C17</f>
         <v>348752915.52607417</v>
       </c>
     </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B19" s="1"/>
-      <c r="C19" s="2"/>
-    </row>
-    <row r="30" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B30" s="5" t="s">
+    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B20" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C30" s="4">
+      <c r="C20" s="2">
         <v>33.1</v>
       </c>
     </row>
-    <row r="31" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B31" s="5" t="s">
+    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B21" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C31" s="4">
+      <c r="C21" s="2">
         <v>145.30000000000001</v>
       </c>
     </row>
-    <row r="32" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B32" s="5" t="s">
+    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B22" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C32" s="4">
+      <c r="C22" s="2">
         <v>605</v>
       </c>
     </row>

</xml_diff>